<commit_message>
Replaced with echurchill default 1.13 friendly build 3.21
</commit_message>
<xml_diff>
--- a/notes/Range Calculation.xlsx
+++ b/notes/Range Calculation.xlsx
@@ -1,26 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eddie\git\CityWorld\notes\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="96" yWindow="48" windowWidth="17220" windowHeight="9000" activeTab="3"/>
+    <workbookView xWindow="90" yWindow="45" windowWidth="17220" windowHeight="9000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="ValueRange">Sheet1!$U$5:$U$8</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="17">
   <si>
     <t>-1 to 1</t>
   </si>
@@ -63,12 +69,21 @@
   <si>
     <t>Foothill</t>
   </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,6 +101,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -113,7 +136,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -122,12 +145,84 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="11">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -153,6 +248,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -201,7 +299,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -236,7 +334,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -451,13 +549,13 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="7" max="7" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="7" max="7" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -496,7 +594,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -546,7 +644,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f>A2-0.05</f>
         <v>0.95</v>
@@ -591,7 +689,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <f t="shared" ref="A4:A42" si="8">A3-0.05</f>
         <v>0.89999999999999991</v>
@@ -645,7 +743,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f t="shared" si="8"/>
         <v>0.84999999999999987</v>
@@ -709,7 +807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f t="shared" si="8"/>
         <v>0.79999999999999982</v>
@@ -774,7 +872,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f t="shared" si="8"/>
         <v>0.74999999999999978</v>
@@ -838,7 +936,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f t="shared" si="8"/>
         <v>0.69999999999999973</v>
@@ -902,7 +1000,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f t="shared" si="8"/>
         <v>0.64999999999999969</v>
@@ -947,7 +1045,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f t="shared" si="8"/>
         <v>0.59999999999999964</v>
@@ -992,7 +1090,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f t="shared" si="8"/>
         <v>0.5499999999999996</v>
@@ -1037,7 +1135,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <f t="shared" si="8"/>
         <v>0.49999999999999961</v>
@@ -1082,7 +1180,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <f t="shared" si="8"/>
         <v>0.44999999999999962</v>
@@ -1127,7 +1225,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <f t="shared" si="8"/>
         <v>0.39999999999999963</v>
@@ -1172,7 +1270,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <f t="shared" si="8"/>
         <v>0.34999999999999964</v>
@@ -1220,7 +1318,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <f t="shared" si="8"/>
         <v>0.29999999999999966</v>
@@ -1272,7 +1370,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <f t="shared" si="8"/>
         <v>0.24999999999999967</v>
@@ -1324,7 +1422,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <f t="shared" si="8"/>
         <v>0.19999999999999968</v>
@@ -1376,7 +1474,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <f t="shared" si="8"/>
         <v>0.14999999999999969</v>
@@ -1428,7 +1526,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <f t="shared" si="8"/>
         <v>9.9999999999999686E-2</v>
@@ -1473,7 +1571,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <f t="shared" si="8"/>
         <v>4.9999999999999684E-2</v>
@@ -1518,7 +1616,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <f t="shared" si="8"/>
         <v>-3.1918911957973251E-16</v>
@@ -1563,7 +1661,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <f t="shared" si="8"/>
         <v>-5.0000000000000322E-2</v>
@@ -1608,7 +1706,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <f t="shared" si="8"/>
         <v>-0.10000000000000032</v>
@@ -1653,7 +1751,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <f t="shared" si="8"/>
         <v>-0.15000000000000033</v>
@@ -1698,7 +1796,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <f t="shared" si="8"/>
         <v>-0.20000000000000034</v>
@@ -1746,7 +1844,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <f t="shared" si="8"/>
         <v>-0.25000000000000033</v>
@@ -1798,7 +1896,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <f t="shared" si="8"/>
         <v>-0.30000000000000032</v>
@@ -1850,7 +1948,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <f t="shared" si="8"/>
         <v>-0.35000000000000031</v>
@@ -1902,7 +2000,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <f t="shared" si="8"/>
         <v>-0.4000000000000003</v>
@@ -1947,7 +2045,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <f t="shared" si="8"/>
         <v>-0.45000000000000029</v>
@@ -1992,7 +2090,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <f t="shared" si="8"/>
         <v>-0.50000000000000033</v>
@@ -2037,7 +2135,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <f t="shared" si="8"/>
         <v>-0.55000000000000038</v>
@@ -2082,7 +2180,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <f t="shared" si="8"/>
         <v>-0.60000000000000042</v>
@@ -2136,7 +2234,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <f t="shared" si="8"/>
         <v>-0.65000000000000047</v>
@@ -2178,7 +2276,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <f t="shared" si="8"/>
         <v>-0.70000000000000051</v>
@@ -2220,7 +2318,7 @@
         <v>-16</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <f t="shared" si="8"/>
         <v>-0.75000000000000056</v>
@@ -2262,7 +2360,7 @@
         <v>-24</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <f t="shared" si="8"/>
         <v>-0.8000000000000006</v>
@@ -2304,7 +2402,7 @@
         <v>-32</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <f t="shared" si="8"/>
         <v>-0.85000000000000064</v>
@@ -2346,7 +2444,7 @@
         <v>-40</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <f t="shared" si="8"/>
         <v>-0.90000000000000069</v>
@@ -2388,7 +2486,7 @@
         <v>-48</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <f t="shared" si="8"/>
         <v>-0.95000000000000073</v>
@@ -2430,7 +2528,7 @@
         <v>-56</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <f t="shared" si="8"/>
         <v>-1.0000000000000007</v>
@@ -2474,12 +2572,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:E1048576">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:Q1">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2490,15 +2588,610 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B12:BQ14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="2.85546875" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="12" spans="2:69" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M12" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="N12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="O12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="P12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="R12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="S12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="T12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="U12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="V12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="W12" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="X12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AK12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AL12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AM12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AN12" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="AO12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AP12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AQ12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AR12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AS12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AT12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AU12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AV12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AW12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AX12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AY12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AZ12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="BA12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="BB12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="BC12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="BD12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="BE12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="BF12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="BG12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="BH12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="BI12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="BJ12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="BK12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="BL12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="BM12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="BN12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="BO12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="BP12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="BQ12" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="2:69" x14ac:dyDescent="0.25">
+      <c r="B13" s="7">
+        <v>0</v>
+      </c>
+      <c r="C13" s="7">
+        <f>B13+1</f>
+        <v>1</v>
+      </c>
+      <c r="D13" s="7">
+        <f t="shared" ref="D13:BO13" si="0">C13+1</f>
+        <v>2</v>
+      </c>
+      <c r="E13" s="7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F13" s="7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G13" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H13" s="7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="I13" s="7">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="J13" s="7">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="K13" s="7">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="L13" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="M13" s="7">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="N13" s="7">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="O13" s="7">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="P13" s="7">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="Q13" s="7">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="R13" s="7">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="S13" s="7">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="T13" s="7">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="U13" s="7">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="V13" s="7">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="W13" s="7">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="X13" s="7">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="Y13" s="7">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="Z13" s="7">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="AA13" s="7">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="AB13" s="7">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="AC13" s="7">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="AD13" s="7">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="AE13" s="7">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="AF13" s="7">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="AG13" s="7">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="AH13" s="7">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="AI13" s="7">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="AJ13" s="7">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="AK13" s="7">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="AL13" s="7">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="AM13" s="7">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="AN13" s="7">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="AO13" s="7">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="AP13" s="7">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="AQ13" s="7">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="AR13" s="7">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="AS13" s="7">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="AT13" s="7">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="AU13" s="7">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="AV13" s="7">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="AW13" s="7">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="AX13" s="7">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="AY13" s="7">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="AZ13" s="7">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="BA13" s="7">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="BB13" s="7">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="BC13" s="7">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="BD13" s="7">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="BE13" s="7">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="BF13" s="7">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="BG13" s="7">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="BH13" s="7">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="BI13" s="7">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="BJ13" s="7">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="BK13" s="7">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="BL13" s="7">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="BM13" s="7">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="BN13" s="7">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="BO13" s="7">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="BP13" s="7">
+        <f t="shared" ref="BP13:BQ13" si="1">BO13+1</f>
+        <v>66</v>
+      </c>
+      <c r="BQ13" s="7">
+        <f t="shared" si="1"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="2:69" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M14" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="O14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="P14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="R14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="S14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="T14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="U14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="V14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="W14" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="X14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AK14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AL14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AM14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AN14" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:XFD1048576">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+      <formula>"R"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+      <formula>"B"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1">
         <v>65</v>
       </c>
@@ -2506,7 +3199,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>14</v>
       </c>
@@ -2519,7 +3212,7 @@
         <v>200.86153846153846</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>16</v>
       </c>
@@ -2532,7 +3225,7 @@
         <v>192.98461538461538</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>30</v>
       </c>
@@ -2545,7 +3238,7 @@
         <v>137.84615384615384</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>32</v>
       </c>
@@ -2558,7 +3251,7 @@
         <v>129.96923076923076</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>65</v>
       </c>
@@ -2576,7 +3269,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D42"/>
   <sheetViews>
@@ -2584,12 +3277,12 @@
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1">
         <v>0.33</v>
       </c>
@@ -2598,7 +3291,7 @@
         <v>0.66999999999999993</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="1">
         <v>1</v>
       </c>
@@ -2607,7 +3300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <f>B2-0.05</f>
         <v>0.95</v>
@@ -2617,7 +3310,7 @@
         <v>0.9253731343283581</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <f t="shared" ref="B4:B42" si="1">B3-0.05</f>
         <v>0.89999999999999991</v>
@@ -2627,7 +3320,7 @@
         <v>0.85074626865671632</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <f t="shared" si="1"/>
         <v>0.84999999999999987</v>
@@ -2637,7 +3330,7 @@
         <v>0.77611940298507442</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <f t="shared" si="1"/>
         <v>0.79999999999999982</v>
@@ -2647,7 +3340,7 @@
         <v>0.70149253731343264</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <f t="shared" si="1"/>
         <v>0.74999999999999978</v>
@@ -2657,7 +3350,7 @@
         <v>0.62686567164179074</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <f t="shared" si="1"/>
         <v>0.69999999999999973</v>
@@ -2667,7 +3360,7 @@
         <v>0.55223880597014885</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <f t="shared" si="1"/>
         <v>0.64999999999999969</v>
@@ -2677,7 +3370,7 @@
         <v>0.47761194029850701</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <f t="shared" si="1"/>
         <v>0.59999999999999964</v>
@@ -2687,7 +3380,7 @@
         <v>0.40298507462686517</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <f t="shared" si="1"/>
         <v>0.5499999999999996</v>
@@ -2697,7 +3390,7 @@
         <v>0.32835820895522327</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <f t="shared" si="1"/>
         <v>0.49999999999999961</v>
@@ -2707,7 +3400,7 @@
         <v>0.25373134328358149</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <f t="shared" si="1"/>
         <v>0.44999999999999962</v>
@@ -2717,7 +3410,7 @@
         <v>0.17910447761193973</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <f t="shared" si="1"/>
         <v>0.39999999999999963</v>
@@ -2727,7 +3420,7 @@
         <v>0.10447761194029795</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <f t="shared" si="1"/>
         <v>0.34999999999999964</v>
@@ -2737,7 +3430,7 @@
         <v>2.9850746268656168E-2</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <f t="shared" si="1"/>
         <v>0.29999999999999966</v>
@@ -2747,7 +3440,7 @@
         <v>-4.4776119402985613E-2</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <f t="shared" si="1"/>
         <v>0.24999999999999967</v>
@@ -2757,7 +3450,7 @@
         <v>-0.1194029850746274</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <f t="shared" si="1"/>
         <v>0.19999999999999968</v>
@@ -2767,7 +3460,7 @@
         <v>-0.19402985074626919</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <f t="shared" si="1"/>
         <v>0.14999999999999969</v>
@@ -2777,7 +3470,7 @@
         <v>-0.26865671641791095</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <f t="shared" si="1"/>
         <v>9.9999999999999686E-2</v>
@@ -2787,7 +3480,7 @@
         <v>-0.34328358208955273</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <f t="shared" si="1"/>
         <v>4.9999999999999684E-2</v>
@@ -2797,7 +3490,7 @@
         <v>-0.41791044776119463</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <f t="shared" si="1"/>
         <v>-3.1918911957973251E-16</v>
@@ -2807,7 +3500,7 @@
         <v>-0.49253731343283641</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <f t="shared" si="1"/>
         <v>-5.0000000000000322E-2</v>
@@ -2817,7 +3510,7 @@
         <v>-0.56716417910447814</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
         <f t="shared" si="1"/>
         <v>-0.10000000000000032</v>
@@ -2827,7 +3520,7 @@
         <v>-0.64179104477611992</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
         <f t="shared" si="1"/>
         <v>-0.15000000000000033</v>
@@ -2837,7 +3530,7 @@
         <v>-0.71641791044776171</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
         <f t="shared" si="1"/>
         <v>-0.20000000000000034</v>
@@ -2847,7 +3540,7 @@
         <v>-0.7910447761194036</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
         <f t="shared" si="1"/>
         <v>-0.25000000000000033</v>
@@ -2857,7 +3550,7 @@
         <v>-0.86567164179104528</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
         <f t="shared" si="1"/>
         <v>-0.30000000000000032</v>
@@ -2867,7 +3560,7 @@
         <v>-0.94029850746268717</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="1">
         <f t="shared" si="1"/>
         <v>-0.35000000000000031</v>
@@ -2877,7 +3570,7 @@
         <v>-1.0149253731343291</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="1">
         <f t="shared" si="1"/>
         <v>-0.4000000000000003</v>
@@ -2887,7 +3580,7 @@
         <v>-1.0895522388059706</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="1">
         <f t="shared" si="1"/>
         <v>-0.45000000000000029</v>
@@ -2897,7 +3590,7 @@
         <v>-1.1641791044776124</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" s="1">
         <f t="shared" si="1"/>
         <v>-0.50000000000000033</v>
@@ -2907,7 +3600,7 @@
         <v>-1.2388059701492542</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="1">
         <f t="shared" si="1"/>
         <v>-0.55000000000000038</v>
@@ -2917,7 +3610,7 @@
         <v>-1.3134328358208962</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" s="1">
         <f t="shared" si="1"/>
         <v>-0.60000000000000042</v>
@@ -2927,7 +3620,7 @@
         <v>-1.388059701492538</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" s="1">
         <f t="shared" si="1"/>
         <v>-0.65000000000000047</v>
@@ -2937,7 +3630,7 @@
         <v>-1.46268656716418</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" s="1">
         <f t="shared" si="1"/>
         <v>-0.70000000000000051</v>
@@ -2947,7 +3640,7 @@
         <v>-1.5373134328358218</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" s="1">
         <f t="shared" si="1"/>
         <v>-0.75000000000000056</v>
@@ -2957,7 +3650,7 @@
         <v>-1.6119402985074636</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" s="1">
         <f t="shared" si="1"/>
         <v>-0.8000000000000006</v>
@@ -2967,7 +3660,7 @@
         <v>-1.6865671641791056</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" s="1">
         <f t="shared" si="1"/>
         <v>-0.85000000000000064</v>
@@ -2977,7 +3670,7 @@
         <v>-1.7611940298507474</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" s="1">
         <f t="shared" si="1"/>
         <v>-0.90000000000000069</v>
@@ -2987,7 +3680,7 @@
         <v>-1.8358208955223891</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" s="1">
         <f t="shared" si="1"/>
         <v>-0.95000000000000073</v>
@@ -2997,7 +3690,7 @@
         <v>-1.9104477611940311</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" s="1">
         <f t="shared" si="1"/>
         <v>-1.0000000000000007</v>
@@ -3012,222 +3705,222 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <f ca="1">RANDBETWEEN(0,255)</f>
-        <v>198</v>
+        <v>255</v>
       </c>
       <c r="B2">
         <f ca="1">AVERAGE(A2:A21)</f>
-        <v>143.30000000000001</v>
+        <v>122.8</v>
       </c>
       <c r="C2">
         <f ca="1">A2</f>
-        <v>198</v>
+        <v>255</v>
       </c>
       <c r="D2">
         <f ca="1">SUM(A2:A21)/COUNT(A2:A21)</f>
-        <v>143.30000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>122.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ref="A3:A21" ca="1" si="0">RANDBETWEEN(0,255)</f>
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C21" ca="1" si="1">(A3+C2)/2</f>
-        <v>116</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>172.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>73</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="1"/>
-        <v>68.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>122.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ca="1" si="0"/>
-        <v>219</v>
+        <v>139</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="1"/>
-        <v>143.75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>130.875</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ca="1" si="0"/>
-        <v>253</v>
+        <v>95</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="1"/>
-        <v>198.375</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>112.9375</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ca="1" si="0"/>
-        <v>245</v>
+        <v>107</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="1"/>
-        <v>221.6875</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>109.96875</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" ca="1" si="0"/>
-        <v>69</v>
+        <v>178</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="1"/>
-        <v>145.34375</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>143.984375</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" ca="1" si="0"/>
-        <v>249</v>
+        <v>213</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="1"/>
-        <v>197.171875</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>178.4921875</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" ca="1" si="0"/>
-        <v>82</v>
+        <v>148</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="1"/>
-        <v>139.5859375</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>163.24609375</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" ca="1" si="0"/>
-        <v>213</v>
+        <v>146</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="1"/>
-        <v>176.29296875</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>154.623046875</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" ca="1" si="0"/>
-        <v>192</v>
+        <v>57</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="1"/>
-        <v>184.146484375</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>105.8115234375</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" ca="1" si="0"/>
-        <v>215</v>
+        <v>240</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="1"/>
-        <v>199.5732421875</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>172.90576171875</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" ca="1" si="0"/>
-        <v>254</v>
+        <v>50</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="1"/>
-        <v>226.78662109375</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>111.452880859375</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" ca="1" si="0"/>
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="1"/>
-        <v>163.893310546875</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>101.7264404296875</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" ca="1" si="0"/>
-        <v>199</v>
+        <v>56</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="1"/>
-        <v>181.4466552734375</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>78.86322021484375</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" ca="1" si="0"/>
-        <v>102</v>
+        <v>224</v>
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
-        <v>141.72332763671875</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>151.43161010742188</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" ca="1" si="0"/>
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
-        <v>96.361663818359375</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+        <v>81.715805053710938</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
-        <v>56.180831909179688</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+        <v>68.357902526855469</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" ca="1" si="0"/>
-        <v>77</v>
+        <v>203</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="1"/>
-        <v>66.590415954589844</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+        <v>135.67895126342773</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" ca="1" si="0"/>
-        <v>76</v>
+        <v>23</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="1"/>
-        <v>71.295207977294922</v>
+        <v>79.339475631713867</v>
       </c>
     </row>
   </sheetData>

</xml_diff>